<commit_message>
feat: method = en-greedy
</commit_message>
<xml_diff>
--- a/Ejemplo Q_learning.xlsx
+++ b/Ejemplo Q_learning.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://alumnosuaicl-my.sharepoint.com/personal/rabarza_alumnos_uai_cl/Documents/UNIVERSIDAD/MAGÍSTER/Temas de Investigación/Tema de Investigación - M. Bravo y F. Lagos/Q Learning/Implementacion/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roloa\OneDrive - Universidad Adolfo Ibanez\UNIVERSIDAD\MAGÍSTER\Temas de Investigación\Tema de Investigación - M. Bravo y F. Lagos\Q Learning\Implementacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6C78C8E0-5736-44DF-B581-CF60A779CE99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4636D450-19B1-4FA4-8534-42E5414780FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16354" yWindow="-2923" windowWidth="22149" windowHeight="13920" xr2:uid="{0034A910-68DD-45D9-8268-71F3ECF82998}"/>
+    <workbookView minimized="1" xWindow="-21566" yWindow="-214" windowWidth="21652" windowHeight="11863" xr2:uid="{0034A910-68DD-45D9-8268-71F3ECF82998}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -94,7 +94,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -112,6 +112,16 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -427,7 +437,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -435,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF2E1944-6783-4739-9D9C-A3EB8E1BDF3F}">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -765,13 +775,341 @@
         <v>-100</v>
       </c>
     </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B12" cm="1">
+        <f t="array" ref="B12:J12">TRANSPOSE(A13:A21)</f>
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12">
+        <v>3</v>
+      </c>
+      <c r="E12">
+        <v>4</v>
+      </c>
+      <c r="F12">
+        <v>5</v>
+      </c>
+      <c r="G12">
+        <v>6</v>
+      </c>
+      <c r="H12">
+        <v>7</v>
+      </c>
+      <c r="I12">
+        <v>8</v>
+      </c>
+      <c r="J12">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13">
+        <v>-100</v>
+      </c>
+      <c r="C13">
+        <v>-100</v>
+      </c>
+      <c r="D13">
+        <v>-100</v>
+      </c>
+      <c r="E13">
+        <v>-100</v>
+      </c>
+      <c r="F13">
+        <v>-100</v>
+      </c>
+      <c r="G13">
+        <v>-100</v>
+      </c>
+      <c r="H13">
+        <v>-100</v>
+      </c>
+      <c r="I13">
+        <v>-100</v>
+      </c>
+      <c r="J13">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>2</v>
+      </c>
+      <c r="B14">
+        <v>-1</v>
+      </c>
+      <c r="C14">
+        <v>-1</v>
+      </c>
+      <c r="D14">
+        <v>-1</v>
+      </c>
+      <c r="E14">
+        <v>-1</v>
+      </c>
+      <c r="F14">
+        <v>-1</v>
+      </c>
+      <c r="G14">
+        <v>-1</v>
+      </c>
+      <c r="H14">
+        <v>-100</v>
+      </c>
+      <c r="I14">
+        <v>-1</v>
+      </c>
+      <c r="J14">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>3</v>
+      </c>
+      <c r="B15">
+        <v>-100</v>
+      </c>
+      <c r="C15">
+        <v>-100</v>
+      </c>
+      <c r="D15">
+        <v>-100</v>
+      </c>
+      <c r="E15">
+        <v>-1</v>
+      </c>
+      <c r="F15">
+        <v>-100</v>
+      </c>
+      <c r="G15">
+        <v>-100</v>
+      </c>
+      <c r="H15">
+        <v>-100</v>
+      </c>
+      <c r="I15">
+        <v>-1</v>
+      </c>
+      <c r="J15">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>4</v>
+      </c>
+      <c r="B16">
+        <v>-100</v>
+      </c>
+      <c r="C16">
+        <v>-1</v>
+      </c>
+      <c r="D16">
+        <v>-1</v>
+      </c>
+      <c r="E16">
+        <v>-1</v>
+      </c>
+      <c r="F16">
+        <v>-100</v>
+      </c>
+      <c r="G16">
+        <v>-1</v>
+      </c>
+      <c r="H16">
+        <v>-100</v>
+      </c>
+      <c r="I16">
+        <v>-1</v>
+      </c>
+      <c r="J16">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>5</v>
+      </c>
+      <c r="B17">
+        <v>-100</v>
+      </c>
+      <c r="C17">
+        <v>-1</v>
+      </c>
+      <c r="D17">
+        <v>-100</v>
+      </c>
+      <c r="E17">
+        <v>-100</v>
+      </c>
+      <c r="F17">
+        <v>-100</v>
+      </c>
+      <c r="G17">
+        <v>-1</v>
+      </c>
+      <c r="H17">
+        <v>-100</v>
+      </c>
+      <c r="I17">
+        <v>-1</v>
+      </c>
+      <c r="J17">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>6</v>
+      </c>
+      <c r="B18">
+        <v>-100</v>
+      </c>
+      <c r="C18">
+        <v>-1</v>
+      </c>
+      <c r="D18">
+        <v>-1</v>
+      </c>
+      <c r="E18">
+        <v>-1</v>
+      </c>
+      <c r="F18">
+        <v>-1</v>
+      </c>
+      <c r="G18">
+        <v>-1</v>
+      </c>
+      <c r="H18">
+        <v>-1</v>
+      </c>
+      <c r="I18">
+        <v>-1</v>
+      </c>
+      <c r="J18">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>7</v>
+      </c>
+      <c r="B19">
+        <v>-100</v>
+      </c>
+      <c r="C19">
+        <v>-1</v>
+      </c>
+      <c r="D19">
+        <v>-100</v>
+      </c>
+      <c r="E19">
+        <v>-100</v>
+      </c>
+      <c r="F19">
+        <v>-100</v>
+      </c>
+      <c r="G19">
+        <v>-1</v>
+      </c>
+      <c r="H19">
+        <v>-100</v>
+      </c>
+      <c r="I19">
+        <v>-1</v>
+      </c>
+      <c r="J19">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>8</v>
+      </c>
+      <c r="B20">
+        <v>-1</v>
+      </c>
+      <c r="C20">
+        <v>-1</v>
+      </c>
+      <c r="D20">
+        <v>-100</v>
+      </c>
+      <c r="E20">
+        <v>-1</v>
+      </c>
+      <c r="F20">
+        <v>-1</v>
+      </c>
+      <c r="G20">
+        <v>-1</v>
+      </c>
+      <c r="H20">
+        <v>-100</v>
+      </c>
+      <c r="I20">
+        <v>-1</v>
+      </c>
+      <c r="J20">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>9</v>
+      </c>
+      <c r="B21">
+        <v>-100</v>
+      </c>
+      <c r="C21">
+        <v>-100</v>
+      </c>
+      <c r="D21">
+        <v>-100</v>
+      </c>
+      <c r="E21">
+        <v>-100</v>
+      </c>
+      <c r="F21">
+        <v>-100</v>
+      </c>
+      <c r="G21">
+        <v>-100</v>
+      </c>
+      <c r="H21">
+        <v>-100</v>
+      </c>
+      <c r="I21">
+        <v>-100</v>
+      </c>
+      <c r="J21">
+        <v>-100</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="B2:J10">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>-100</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+      <formula>500</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B13:J21">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>-100</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J15">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>500</formula>
     </cfRule>

</xml_diff>